<commit_message>
Cambios para que funcione la strategy limits en el arranque
</commit_message>
<xml_diff>
--- a/Stock/Valores IBEX.xlsx
+++ b/Stock/Valores IBEX.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores IBEX" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1038,19 +1038,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1063,10 +1065,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>